<commit_message>
[FEATURE]: paths and libraries added
</commit_message>
<xml_diff>
--- a/CRIS_single-sample/src/utils/paths_db.xlsx
+++ b/CRIS_single-sample/src/utils/paths_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\Desktop\CRIS_single-sample\CRIS_single-sample\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC36EB6E-122F-4BBF-AF72-59C86AEEF07C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5229C82C-4A2B-4F7C-A002-9A64441FBDF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17412" yWindow="3696" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
   <si>
     <t>label</t>
   </si>
@@ -54,30 +54,12 @@
     <t>GMQL_GRCH38_ANNOT</t>
   </si>
   <si>
-    <t>data/source_data/GMQL_GRCH38/GMQL_GRCH38.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/GMQL_GRCH38/GMQL_GRCH38_FILTERED_unif.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/GMQL_GRCH38/GMQL_GRCH38_FILTERED.rds</t>
-  </si>
-  <si>
     <t>GMQL_GRCH38_FILT_UNIF</t>
   </si>
   <si>
-    <t>data/source_data/GMQL_GRCH38/annotations/gmql_grch38_metadata.xlsx</t>
-  </si>
-  <si>
-    <t>data/source_data/GMQL_GRCH38/annotations/gmql_grch38_annotations.xlsx</t>
-  </si>
-  <si>
     <t>CANDIOLO_HG19</t>
   </si>
   <si>
-    <t>data/source_data/CANDIOLO_HG19/CANDIOLO_HG19.rds</t>
-  </si>
-  <si>
     <t>PDX_1</t>
   </si>
   <si>
@@ -96,36 +78,6 @@
     <t>PDX_6</t>
   </si>
   <si>
-    <t>data/source_data/PDX/Hbiod1_LMX.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod2_LMX.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod3_LMX.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod4_LMX.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod5_LMX.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod6_LMX.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod1_LMX_FILTERED.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod2_LMX_FILTERED.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod3_LMX_FILTERED.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod4_LMX_FILTERED.rds</t>
-  </si>
-  <si>
     <t>PDX_MERGED_FILT</t>
   </si>
   <si>
@@ -135,9 +87,6 @@
     <t>PDX_MERGED_ANNOT</t>
   </si>
   <si>
-    <t>data/source_data/PDX/annotations/pdx_grch38_annotations.xlsx</t>
-  </si>
-  <si>
     <t>PDX_1_FILTERED</t>
   </si>
   <si>
@@ -156,10 +105,163 @@
     <t>PDX_6_FILTERED</t>
   </si>
   <si>
-    <t>data/source_data/PDX/Hbiod_MERGED_FILTERED.rds</t>
-  </si>
-  <si>
-    <t>data/source_data/PDX/Hbiod_MERGED_FILTERED_unif.rds</t>
+    <t>NTP_REF_TCGA</t>
+  </si>
+  <si>
+    <t>NTP_REF_PDX</t>
+  </si>
+  <si>
+    <t>data/references/NTP_cpm_tcga_reference.rds</t>
+  </si>
+  <si>
+    <t>data/references/NTP_cpm_pdx_reference.rds</t>
+  </si>
+  <si>
+    <t>FEATURES_HG19</t>
+  </si>
+  <si>
+    <t>FEATURES_GRCH38</t>
+  </si>
+  <si>
+    <t>FEATURES_PDX</t>
+  </si>
+  <si>
+    <t>FEATURES_ORIGINAL</t>
+  </si>
+  <si>
+    <t>data/genes/ntp_signature_tcga_hg19_original.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/ntp_signature_tcga_hg19_filtered.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/ntp_signature_tcga_grch38.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/ntp_signature_pdx_grch38.xlsx</t>
+  </si>
+  <si>
+    <t>TCGA_SPLITTING</t>
+  </si>
+  <si>
+    <t>data/references/tcga_splitting.xlsx</t>
+  </si>
+  <si>
+    <t>PUB_TSP</t>
+  </si>
+  <si>
+    <t>PUB_NTP</t>
+  </si>
+  <si>
+    <t>data/references/published_ntp.xlsx</t>
+  </si>
+  <si>
+    <t>data/references/published_tsp.xlsx</t>
+  </si>
+  <si>
+    <t>NTP_THR</t>
+  </si>
+  <si>
+    <t>data/references/ml_ntp_thresholds.rds</t>
+  </si>
+  <si>
+    <t>HD_PDX</t>
+  </si>
+  <si>
+    <t>BIO_LASSO_TCGA</t>
+  </si>
+  <si>
+    <t>BIO_LASSO_PDX</t>
+  </si>
+  <si>
+    <t>BIO_DRIVEN_TCGA</t>
+  </si>
+  <si>
+    <t>data/genes/feature_selection/bio_driven_lasso_tcga_robust_union.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/feature_selection/bio_driven_lasso_pdx_robust_union.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/feature_selection/bio_fs_genes_tcga.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/feature_selection/bio_fs_genes_pdx.xlsx</t>
+  </si>
+  <si>
+    <t>BIO_DRIVEN_PDX</t>
+  </si>
+  <si>
+    <t>data/genes/entrez_corr_pdx.xlsx</t>
+  </si>
+  <si>
+    <t>data/genes/entrez_corr_tcga.xlsx</t>
+  </si>
+  <si>
+    <t>ENTREZ_CORR_TCGA</t>
+  </si>
+  <si>
+    <t>ENTREZ_CORR_PDX</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_hg19/CANDIOLO_HG19.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_GRCh38/TCGA_RNAseq_GRCh38.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_GRCh38/GMQL_GRCH38_FILTERED.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_GRCh38/GMQL_GRCH38_FILTERED_unif.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_GRCh38/annotations/gmql_grch38_metadata.xlsx</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_GRCh38/annotations/gmql_grch38_annotations.xlsx</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod1_LMX.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod2_LMX.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod3_LMX.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod4_LMX.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod5_LMX.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod6_LMX.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod1_LMX_FILTERED.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod2_LMX_FILTERED.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod3_LMX_FILTERED.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod4_LMX_FILTERED.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod_MERGED_FILTERED.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/Hbiod_MERGED_FILTERED_unif.rds</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/PDX_GRCH38/annotations/pdx_grch38_annotations.xlsx</t>
+  </si>
+  <si>
+    <t>data/source_data/PDX_RNAseq_GRCh38/HIGH_DEPTH_PDX_GRCH38/high_depth_LMX_samples.xlsx</t>
   </si>
 </sst>
 </file>
@@ -523,15 +625,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="79.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -545,170 +647,306 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[REFACTOR]: documentation comments on data classes and debug
Path_db correction and missing source added in vignette
</commit_message>
<xml_diff>
--- a/CRIS_single-sample/src/utils/paths_db.xlsx
+++ b/CRIS_single-sample/src/utils/paths_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\Desktop\CRIS_single-sample\CRIS_single-sample\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5229C82C-4A2B-4F7C-A002-9A64441FBDF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0AE88C-701D-4A65-A1A4-77E118FC4283}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17412" yWindow="3696" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1992" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>data/source_data/TCGA_RNAseq_hg19/CANDIOLO_HG19.rds</t>
   </si>
   <si>
-    <t>data/source_data/TCGA_RNAseq_GRCh38/TCGA_RNAseq_GRCh38.rds</t>
-  </si>
-  <si>
     <t>data/source_data/TCGA_RNAseq_GRCh38/GMQL_GRCH38_FILTERED.rds</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>data/source_data/PDX_RNAseq_GRCh38/HIGH_DEPTH_PDX_GRCH38/high_depth_LMX_samples.xlsx</t>
+  </si>
+  <si>
+    <t>data/source_data/TCGA_RNAseq_GRCh38/GMQL_GRCh38.rds</t>
   </si>
 </sst>
 </file>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -674,7 +674,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -682,7 +682,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -690,7 +690,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -698,7 +698,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -706,7 +706,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -714,7 +714,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -722,7 +722,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -730,7 +730,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -738,7 +738,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -746,7 +746,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -762,7 +762,7 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -770,7 +770,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -778,7 +778,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -786,7 +786,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -794,7 +794,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -802,7 +802,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -810,7 +810,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -898,7 +898,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[SCRIPT]: script for training of all single-label classifiers
</commit_message>
<xml_diff>
--- a/CRIS_single-sample/src/utils/paths_db.xlsx
+++ b/CRIS_single-sample/src/utils/paths_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\Desktop\CRIS_single-sample\CRIS_single-sample\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0AE88C-701D-4A65-A1A4-77E118FC4283}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3897AA89-520D-44AD-8BC1-9C4D250E32AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1992" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>label</t>
   </si>
@@ -262,13 +262,19 @@
   </si>
   <si>
     <t>data/source_data/TCGA_RNAseq_GRCh38/GMQL_GRCh38.rds</t>
+  </si>
+  <si>
+    <t>OUT_FOLDER_MODELS</t>
+  </si>
+  <si>
+    <t>data/classifiers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +284,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -305,12 +319,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -625,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,6 +964,17 @@
         <v>52</v>
       </c>
     </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[SCRIPTS]: ml problem transformation training script
</commit_message>
<xml_diff>
--- a/CRIS_single-sample/src/utils/paths_db.xlsx
+++ b/CRIS_single-sample/src/utils/paths_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\Desktop\CRIS_single-sample\CRIS_single-sample\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3897AA89-520D-44AD-8BC1-9C4D250E32AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443A94A3-408C-4499-A971-72E2FCB16A73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="1476" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -267,7 +267,7 @@
     <t>OUT_FOLDER_MODELS</t>
   </si>
   <si>
-    <t>data/classifiers</t>
+    <t>output/classifiers</t>
   </si>
 </sst>
 </file>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[SCRIPTS]: biological validation and possibility to use published models
</commit_message>
<xml_diff>
--- a/CRIS_single-sample/src/utils/paths_db.xlsx
+++ b/CRIS_single-sample/src/utils/paths_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiar\Desktop\CRIS_single-sample\CRIS_single-sample\src\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443A94A3-408C-4499-A971-72E2FCB16A73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC34E04-E708-4D85-A33C-0E9580454626}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1476" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13824" yWindow="564" windowWidth="17280" windowHeight="9072" tabRatio="323" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t>label</t>
   </si>
@@ -268,6 +268,30 @@
   </si>
   <si>
     <t>output/classifiers</t>
+  </si>
+  <si>
+    <t>NTP_ONLY_SL_MODELS</t>
+  </si>
+  <si>
+    <t>NTP_ONLY_ML_MODELS</t>
+  </si>
+  <si>
+    <t>NTP_ONLY_ML_AA_THR</t>
+  </si>
+  <si>
+    <t>NTP_ONLY_ML_PT_THR</t>
+  </si>
+  <si>
+    <t>data/reference_models/ntp_only/sl_models__tuned.rds</t>
+  </si>
+  <si>
+    <t>data/reference_models/ntp_only/ml_models__tuned.rds</t>
+  </si>
+  <si>
+    <t>data/reference_models/ntp_only/sl_cl_thresholds__tuned.rds</t>
+  </si>
+  <si>
+    <t>data/reference_models/ntp_only/ml_cl_thresholds__tuned.rds</t>
   </si>
 </sst>
 </file>
@@ -640,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +997,42 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
+      <c r="A41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>